<commit_message>
before final update 1
</commit_message>
<xml_diff>
--- a/inputs.xlsx
+++ b/inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m4oughi\Desktop\a\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925649F4-2C85-42F5-AE0B-262964B769E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61302C05-D62F-4E5E-B878-2BC5EBAEA0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Symbol</t>
-  </si>
-  <si>
-    <t>Data</t>
   </si>
   <si>
     <t>noo</t>
@@ -140,15 +137,15 @@
   <si>
     <t>Strips</t>
   </si>
+  <si>
+    <t>Introduction</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +194,20 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -241,7 +252,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -340,15 +351,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -404,7 +406,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -430,30 +432,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
@@ -471,46 +449,86 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="7" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="7" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="7" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="7" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="7" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="7" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="7" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="7" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="7" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="7" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="11" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -724,7 +742,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4736,128 +4753,130 @@
   <dimension ref="A1:AB28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28" style="18" customWidth="1"/>
-    <col min="6" max="9" width="10.109375" style="18" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28" style="10" customWidth="1"/>
+    <col min="6" max="9" width="10.109375" style="10" customWidth="1"/>
     <col min="10" max="10" width="10.33203125" customWidth="1"/>
     <col min="11" max="11" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="29"/>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:24" ht="19.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="40"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="E1" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="32"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:24" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="21">
+      <c r="A2" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="43"/>
+      <c r="C2" s="24">
+        <v>1</v>
+      </c>
+      <c r="D2" s="24">
         <v>0</v>
       </c>
-      <c r="C2" s="21">
+      <c r="E2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="24">
         <v>1</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="21">
-        <v>1</v>
-      </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
     </row>
     <row r="3" spans="1:24" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="21">
+      <c r="A3" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="24">
         <v>0</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
     </row>
     <row r="4" spans="1:24" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
+        <v>37</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="21">
+      <c r="C4" s="3"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="24">
         <v>0</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
-      <c r="V4" s="33"/>
-      <c r="W4" s="33"/>
-      <c r="X4" s="33"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="22"/>
+      <c r="V4" s="22"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
     </row>
     <row r="5" spans="1:24" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="21">
+      <c r="C5" s="24">
         <v>0</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="21">
+      <c r="D5" s="17"/>
+      <c r="E5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="24">
         <v>0</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
       <c r="J5" s="4"/>
       <c r="K5" s="5">
         <v>1</v>
@@ -4903,26 +4922,26 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="18" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="22">
+      <c r="B6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="14">
         <v>70</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="21">
+      <c r="D6" s="17"/>
+      <c r="E6" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="24">
         <v>0</v>
       </c>
-      <c r="G6" s="28"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="36" t="s">
-        <v>37</v>
+      <c r="G6" s="17"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="19" t="s">
+        <v>36</v>
       </c>
       <c r="J6" s="6">
         <v>1</v>
@@ -4971,23 +4990,23 @@
       </c>
     </row>
     <row r="7" spans="1:24" ht="18" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="22">
+      <c r="A7" s="30"/>
+      <c r="B7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="14">
         <v>70</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="21">
+      <c r="D7" s="17"/>
+      <c r="E7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="24">
         <v>0</v>
       </c>
-      <c r="G7" s="28"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="37"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="20"/>
       <c r="J7" s="7">
         <v>2</v>
       </c>
@@ -5035,20 +5054,20 @@
       </c>
     </row>
     <row r="8" spans="1:24" ht="18" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="26">
+      <c r="B8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="24">
         <v>0.3</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="25"/>
-      <c r="I8" s="37"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="16"/>
+      <c r="I8" s="20"/>
       <c r="J8" s="7">
         <v>3</v>
       </c>
@@ -5096,13 +5115,13 @@
       </c>
     </row>
     <row r="9" spans="1:24" ht="18" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="28"/>
-      <c r="I9" s="37"/>
+      <c r="A9" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="35"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="17"/>
+      <c r="I9" s="20"/>
       <c r="J9" s="7">
         <v>4</v>
       </c>
@@ -5150,17 +5169,17 @@
       </c>
     </row>
     <row r="10" spans="1:24" ht="18" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="27">
+      <c r="B10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="24">
         <v>1</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="I10" s="37"/>
+      <c r="D10" s="17"/>
+      <c r="I10" s="20"/>
       <c r="J10" s="7">
         <v>5</v>
       </c>
@@ -5208,129 +5227,129 @@
       </c>
     </row>
     <row r="11" spans="1:24" ht="18" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="27">
+      <c r="A11" s="26"/>
+      <c r="B11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="24">
         <v>1</v>
       </c>
-      <c r="D11" s="28"/>
+      <c r="D11" s="17"/>
     </row>
     <row r="12" spans="1:24" ht="18" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="27">
+      <c r="A12" s="28"/>
+      <c r="B12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="24">
         <v>1E-3</v>
       </c>
-      <c r="D12" s="28"/>
+      <c r="D12" s="17"/>
     </row>
     <row r="13" spans="1:24" ht="18" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="28"/>
+      <c r="A13" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="35"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="17"/>
     </row>
     <row r="14" spans="1:24" ht="18" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="24">
         <v>10</v>
       </c>
-      <c r="D14" s="28"/>
+      <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:24" ht="18" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="19" t="s">
+      <c r="A15" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="14">
         <v>0</v>
       </c>
-      <c r="D15" s="28"/>
+      <c r="D15" s="17"/>
     </row>
     <row r="16" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
-      <c r="B16" s="19" t="s">
+      <c r="A16" s="31"/>
+      <c r="B16" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="14">
         <v>1</v>
       </c>
-      <c r="D16" s="28"/>
+      <c r="D16" s="17"/>
     </row>
     <row r="17" spans="1:28" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="19" t="s">
+      <c r="A17" s="30"/>
+      <c r="B17" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="14">
         <v>0</v>
       </c>
-      <c r="D17" s="28"/>
+      <c r="D17" s="17"/>
     </row>
     <row r="18" spans="1:28" ht="18" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="26">
+      <c r="A18" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="24">
         <v>0</v>
       </c>
-      <c r="D18" s="28"/>
+      <c r="D18" s="17"/>
     </row>
     <row r="19" spans="1:28" ht="18" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="26">
+      <c r="A19" s="28"/>
+      <c r="B19" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="24">
         <v>0</v>
       </c>
-      <c r="D19" s="28"/>
+      <c r="D19" s="17"/>
     </row>
     <row r="20" spans="1:28" ht="18" x14ac:dyDescent="0.3">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="17"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="K21" s="18"/>
+      <c r="K21" s="10"/>
     </row>
     <row r="22" spans="1:28" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K22" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="35"/>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="35"/>
-      <c r="R22" s="35"/>
-      <c r="S22" s="35"/>
-      <c r="T22" s="35"/>
-      <c r="U22" s="35"/>
-      <c r="V22" s="35"/>
-      <c r="W22" s="35"/>
-      <c r="X22" s="35"/>
-      <c r="Y22" s="35"/>
-      <c r="Z22" s="35"/>
-      <c r="AA22" s="35"/>
-      <c r="AB22" s="35"/>
+      <c r="K22" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
+      <c r="U22" s="23"/>
+      <c r="V22" s="23"/>
+      <c r="W22" s="23"/>
+      <c r="X22" s="23"/>
+      <c r="Y22" s="23"/>
+      <c r="Z22" s="23"/>
+      <c r="AA22" s="23"/>
+      <c r="AB22" s="23"/>
     </row>
     <row r="23" spans="1:28" ht="21.6" thickTop="1" x14ac:dyDescent="0.3">
       <c r="K23" s="5">
@@ -5389,8 +5408,8 @@
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="I24" s="36" t="s">
-        <v>37</v>
+      <c r="I24" s="19" t="s">
+        <v>36</v>
       </c>
       <c r="J24" s="6">
         <v>1</v>
@@ -5451,7 +5470,7 @@
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="I25" s="37"/>
+      <c r="I25" s="20"/>
       <c r="J25" s="7">
         <v>2</v>
       </c>
@@ -5511,7 +5530,7 @@
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="I26" s="37"/>
+      <c r="I26" s="20"/>
       <c r="J26" s="7">
         <v>3</v>
       </c>
@@ -5571,7 +5590,7 @@
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="I27" s="37"/>
+      <c r="I27" s="20"/>
       <c r="J27" s="7">
         <v>4</v>
       </c>
@@ -5631,7 +5650,7 @@
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="I28" s="37"/>
+      <c r="I28" s="20"/>
       <c r="J28" s="7">
         <v>5</v>
       </c>
@@ -5691,7 +5710,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="10">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
     <mergeCell ref="I6:I10"/>
     <mergeCell ref="I24:I28"/>
     <mergeCell ref="J4:X4"/>
@@ -5699,10 +5720,7 @@
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A13:C13"/>
     <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>